<commit_message>
Many tweaks. Open to input
We have 8 hrs to fill, the previous version assumed only 6.
</commit_message>
<xml_diff>
--- a/Agenda.xlsx
+++ b/Agenda.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="30" windowWidth="28755" windowHeight="14640"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
   <si>
     <t>Time</t>
   </si>
@@ -27,9 +27,6 @@
     <t>Break</t>
   </si>
   <si>
-    <t>10:30 - 10:40</t>
-  </si>
-  <si>
     <t>Lunch</t>
   </si>
   <si>
@@ -39,51 +36,27 @@
     <t>Review refactored example application</t>
   </si>
   <si>
-    <t>09:00 - 09:15</t>
-  </si>
-  <si>
     <t>Outline agenda, introduction</t>
   </si>
   <si>
     <t>All</t>
   </si>
   <si>
-    <t>09:15 - 09:45</t>
-  </si>
-  <si>
     <t>Presentation: Intro to refactoring, How, When</t>
   </si>
   <si>
     <t>Ryan</t>
   </si>
   <si>
-    <t>Code challenges and discussion</t>
-  </si>
-  <si>
-    <t>Review piece of code as a group and identify bad practices. Use this as a lead-in to present and discuss specific anti-patterns and code smells</t>
-  </si>
-  <si>
-    <t>10:40 - 12:00</t>
-  </si>
-  <si>
-    <t>Continue code challenges and discussion</t>
-  </si>
-  <si>
     <t>Presentation: ?Specific refactoring techniques?</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>1 on 1 code review and refactoring assistance</t>
   </si>
   <si>
     <t>All?</t>
   </si>
   <si>
-    <t>09:30 - 10:30</t>
-  </si>
-  <si>
     <t>12:00 - 01:00</t>
   </si>
   <si>
@@ -96,14 +69,53 @@
     <t>03:00 - 04:00</t>
   </si>
   <si>
-    <t>Take Turns?</t>
+    <t>8:00 - 8:15</t>
+  </si>
+  <si>
+    <t>4:00 - 5:00</t>
+  </si>
+  <si>
+    <t>Cory</t>
+  </si>
+  <si>
+    <t>8:15 - 8:45</t>
+  </si>
+  <si>
+    <t>Code challenges and discussion - Review piece of code as a group and identify bad practices. Use this as a lead-in to present and discuss specific anti-patterns and code smells</t>
+  </si>
+  <si>
+    <t>8:45 - 9:45</t>
+  </si>
+  <si>
+    <t>10:00 - 10:45</t>
+  </si>
+  <si>
+    <t>Refactoring related portions of Clean Code talk</t>
+  </si>
+  <si>
+    <t>10:45 - 12:00</t>
+  </si>
+  <si>
+    <t>Continue challenges and discussions</t>
+  </si>
+  <si>
+    <t>Patrick or Cory</t>
+  </si>
+  <si>
+    <t>Patrick?</t>
+  </si>
+  <si>
+    <t>9:45 - 10:00</t>
+  </si>
+  <si>
+    <t>Review samples from 1 on 1 code reviews with the group.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -140,7 +152,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -155,6 +167,8 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -244,7 +258,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -279,7 +292,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -455,19 +467,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="45.28515625" style="4" customWidth="1"/>
     <col min="3" max="3" width="17.28515625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="3" customFormat="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -475,108 +489,119 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="3" customFormat="1">
+      <c r="A2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="60">
+      <c r="A4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="30">
+      <c r="A11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="B5" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -586,24 +611,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
split good and bad and updated agenda
Oh, and I've reattached my head. Whew!
</commit_message>
<xml_diff>
--- a/Agenda.xlsx
+++ b/Agenda.xlsx
@@ -48,9 +48,6 @@
     <t>Ryan</t>
   </si>
   <si>
-    <t>Presentation: ?Specific refactoring techniques?</t>
-  </si>
-  <si>
     <t>1 on 1 code review and refactoring assistance</t>
   </si>
   <si>
@@ -102,13 +99,16 @@
     <t>Patrick or Cory</t>
   </si>
   <si>
-    <t>Patrick?</t>
-  </si>
-  <si>
     <t>9:45 - 10:00</t>
   </si>
   <si>
     <t>Review samples from 1 on 1 code reviews with the group.</t>
+  </si>
+  <si>
+    <t>Patrick</t>
+  </si>
+  <si>
+    <t>Code smells and Anti-patterns presentation</t>
   </si>
 </sst>
 </file>
@@ -471,7 +471,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -494,18 +494,18 @@
     </row>
     <row r="2" spans="1:3" s="3" customFormat="1">
       <c r="A2" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>8</v>
@@ -516,10 +516,10 @@
     </row>
     <row r="4" spans="1:3" ht="60">
       <c r="A4" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>7</v>
@@ -527,7 +527,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>2</v>
@@ -535,21 +535,21 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>25</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>26</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>7</v>
@@ -557,7 +557,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>3</v>
@@ -565,21 +565,21 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>7</v>
@@ -587,18 +587,18 @@
     </row>
     <row r="11" spans="1:3" ht="30">
       <c r="A11" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
changes to the agenda
</commit_message>
<xml_diff>
--- a/Agenda.xlsx
+++ b/Agenda.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="30" windowWidth="28755" windowHeight="14640"/>
+    <workbookView xWindow="0" yWindow="30" windowWidth="28755" windowHeight="13740"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
   <si>
     <t>Time</t>
   </si>
@@ -33,89 +33,74 @@
     <t>Primary Presenter</t>
   </si>
   <si>
-    <t>Review refactored example application</t>
-  </si>
-  <si>
-    <t>Outline agenda, introduction</t>
-  </si>
-  <si>
     <t>All</t>
   </si>
   <si>
-    <t>Presentation: Intro to refactoring, How, When</t>
-  </si>
-  <si>
     <t>Ryan</t>
   </si>
   <si>
-    <t>1 on 1 code review and refactoring assistance</t>
-  </si>
-  <si>
-    <t>All?</t>
-  </si>
-  <si>
     <t>12:00 - 01:00</t>
   </si>
   <si>
-    <t>01:00 - 01:30</t>
-  </si>
-  <si>
-    <t>01:30 - 03:00</t>
-  </si>
-  <si>
-    <t>03:00 - 04:00</t>
-  </si>
-  <si>
-    <t>8:00 - 8:15</t>
-  </si>
-  <si>
-    <t>4:00 - 5:00</t>
-  </si>
-  <si>
     <t>Cory</t>
   </si>
   <si>
-    <t>8:15 - 8:45</t>
-  </si>
-  <si>
-    <t>Code challenges and discussion - Review piece of code as a group and identify bad practices. Use this as a lead-in to present and discuss specific anti-patterns and code smells</t>
-  </si>
-  <si>
-    <t>8:45 - 9:45</t>
-  </si>
-  <si>
-    <t>10:00 - 10:45</t>
-  </si>
-  <si>
-    <t>Refactoring related portions of Clean Code talk</t>
-  </si>
-  <si>
-    <t>10:45 - 12:00</t>
-  </si>
-  <si>
-    <t>Continue challenges and discussions</t>
-  </si>
-  <si>
-    <t>Patrick or Cory</t>
-  </si>
-  <si>
-    <t>9:45 - 10:00</t>
-  </si>
-  <si>
-    <t>Review samples from 1 on 1 code reviews with the group.</t>
-  </si>
-  <si>
     <t>Patrick</t>
   </si>
   <si>
-    <t>Code smells and Anti-patterns presentation</t>
+    <t>Identifying Code Smells - Discussion and Practice</t>
+  </si>
+  <si>
+    <t>Outline agenda, introduction, attendee code</t>
+  </si>
+  <si>
+    <t>8:00 - 8:45</t>
+  </si>
+  <si>
+    <t>Writing Clean Code</t>
+  </si>
+  <si>
+    <t>1:00-2:00</t>
+  </si>
+  <si>
+    <t>2:00-3:00</t>
+  </si>
+  <si>
+    <t>3:00-3:15</t>
+  </si>
+  <si>
+    <t>8:45-10:00</t>
+  </si>
+  <si>
+    <t>10:00-10:15</t>
+  </si>
+  <si>
+    <t>10:15-12:00</t>
+  </si>
+  <si>
+    <t>Identifying Code Smells - continuation (attendee code)</t>
+  </si>
+  <si>
+    <t>Applying clean code to refactoring (sample app)</t>
+  </si>
+  <si>
+    <t>Refactoring in practice (attendee code)</t>
+  </si>
+  <si>
+    <t>3:15-4:30</t>
+  </si>
+  <si>
+    <t>4:30-5:00</t>
+  </si>
+  <si>
+    <t>Wrap up</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -152,7 +137,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -169,6 +154,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -258,6 +246,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -292,6 +281,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -467,21 +457,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.28515625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="45.140625" style="4" customWidth="1"/>
     <col min="3" max="3" width="17.28515625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="3" customFormat="1">
+    <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -492,116 +482,111 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="3" customFormat="1">
+    <row r="2" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="2" t="s">
-        <v>19</v>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>17</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="60">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" s="4" t="s">
+      <c r="C8" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="2" t="s">
+      <c r="C9" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="2" t="s">
+      <c r="C10" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B11" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="30">
-      <c r="A11" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>28</v>
-      </c>
       <c r="C11" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -611,24 +596,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated agenda and intro power point
</commit_message>
<xml_diff>
--- a/Agenda.xlsx
+++ b/Agenda.xlsx
@@ -39,61 +39,61 @@
     <t>Ryan</t>
   </si>
   <si>
-    <t>12:00 - 01:00</t>
-  </si>
-  <si>
     <t>Cory</t>
   </si>
   <si>
     <t>Patrick</t>
   </si>
   <si>
-    <t>Identifying Code Smells - Discussion and Practice</t>
-  </si>
-  <si>
-    <t>Outline agenda, introduction, attendee code</t>
-  </si>
-  <si>
-    <t>8:00 - 8:45</t>
-  </si>
-  <si>
     <t>Writing Clean Code</t>
   </si>
   <si>
-    <t>1:00-2:00</t>
-  </si>
-  <si>
-    <t>2:00-3:00</t>
-  </si>
-  <si>
-    <t>3:00-3:15</t>
-  </si>
-  <si>
-    <t>8:45-10:00</t>
-  </si>
-  <si>
-    <t>10:00-10:15</t>
-  </si>
-  <si>
-    <t>10:15-12:00</t>
-  </si>
-  <si>
-    <t>Identifying Code Smells - continuation (attendee code)</t>
-  </si>
-  <si>
-    <t>Applying clean code to refactoring (sample app)</t>
-  </si>
-  <si>
-    <t>Refactoring in practice (attendee code)</t>
-  </si>
-  <si>
-    <t>3:15-4:30</t>
-  </si>
-  <si>
-    <t>4:30-5:00</t>
-  </si>
-  <si>
-    <t>Wrap up</t>
+    <t>8am-8:45am</t>
+  </si>
+  <si>
+    <t>Intro</t>
+  </si>
+  <si>
+    <t>8:45am-9:45am</t>
+  </si>
+  <si>
+    <t>Code Smells</t>
+  </si>
+  <si>
+    <t>9:45am-10am</t>
+  </si>
+  <si>
+    <t>10:00am-12pm</t>
+  </si>
+  <si>
+    <t>Code Challenges</t>
+  </si>
+  <si>
+    <t>12pm-1pm</t>
+  </si>
+  <si>
+    <t>1pm-1:45pm</t>
+  </si>
+  <si>
+    <t>1:45pm-2:45pm</t>
+  </si>
+  <si>
+    <t>Refactoring practice and assistance</t>
+  </si>
+  <si>
+    <t>2:45pm-3pm</t>
+  </si>
+  <si>
+    <t>3pm-4pm</t>
+  </si>
+  <si>
+    <t>Attendee code sharing</t>
+  </si>
+  <si>
+    <t>4pm-5pm</t>
+  </si>
+  <si>
+    <t>Conclusions</t>
   </si>
 </sst>
 </file>
@@ -461,12 +461,12 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A2" sqref="A2:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="45.140625" style="4" customWidth="1"/>
     <col min="3" max="3" width="17.28515625" style="2" bestFit="1" customWidth="1"/>
   </cols>
@@ -484,7 +484,7 @@
     </row>
     <row r="2" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>11</v>
@@ -495,18 +495,18 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>2</v>
@@ -515,12 +515,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>5</v>
@@ -528,7 +528,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>3</v>
@@ -536,21 +536,21 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>5</v>
@@ -558,7 +558,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>2</v>
@@ -569,10 +569,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>22</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>5</v>
@@ -586,7 +586,7 @@
         <v>25</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
minor changes to the agenda
</commit_message>
<xml_diff>
--- a/Agenda.xlsx
+++ b/Agenda.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
   <si>
     <t>Time</t>
   </si>
@@ -36,9 +36,6 @@
     <t>All</t>
   </si>
   <si>
-    <t>Ryan</t>
-  </si>
-  <si>
     <t>Cory</t>
   </si>
   <si>
@@ -48,27 +45,12 @@
     <t>Writing Clean Code</t>
   </si>
   <si>
-    <t>8am-8:45am</t>
-  </si>
-  <si>
-    <t>Intro</t>
-  </si>
-  <si>
-    <t>8:45am-9:45am</t>
-  </si>
-  <si>
-    <t>Code Smells</t>
-  </si>
-  <si>
     <t>9:45am-10am</t>
   </si>
   <si>
     <t>10:00am-12pm</t>
   </si>
   <si>
-    <t>Code Challenges</t>
-  </si>
-  <si>
     <t>12pm-1pm</t>
   </si>
   <si>
@@ -78,9 +60,6 @@
     <t>1:45pm-2:45pm</t>
   </si>
   <si>
-    <t>Refactoring practice and assistance</t>
-  </si>
-  <si>
     <t>2:45pm-3pm</t>
   </si>
   <si>
@@ -94,6 +73,21 @@
   </si>
   <si>
     <t>Conclusions</t>
+  </si>
+  <si>
+    <t>8am-9:45am</t>
+  </si>
+  <si>
+    <t>Intro &amp; Calories Calculator App</t>
+  </si>
+  <si>
+    <t>Finding Code Smells</t>
+  </si>
+  <si>
+    <t>Refactoring techniques</t>
+  </si>
+  <si>
+    <t>Ryan &amp; Cory</t>
   </si>
 </sst>
 </file>
@@ -458,16 +452,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B11"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.140625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.5703125" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.28515625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -484,109 +478,98 @@
     </row>
     <row r="2" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>12</v>
+      <c r="A3" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>17</v>
+      <c r="A6" s="8" t="s">
+        <v>12</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>3</v>
+        <v>8</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
-        <v>18</v>
+      <c r="A7" s="5" t="s">
+        <v>13</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>19</v>
+      <c r="A8" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>21</v>
+      <c r="A9" s="5" t="s">
+        <v>15</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>22</v>
+      <c r="A10" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>